<commit_message>
add pdf and excel
</commit_message>
<xml_diff>
--- a/server/clients_export.xlsx
+++ b/server/clients_export.xlsx
@@ -1,17 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6CF096-1699-4D52-916B-182038F787EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="12549" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="63">
+  <si>
+    <t>trash</t>
+  </si>
   <si>
     <t>_id</t>
   </si>
@@ -52,7 +59,34 @@
     <t>123-456-7890</t>
   </si>
   <si>
-    <t>"6591a156d3505b8a202e4c44"</t>
+    <t>"6591a156d3505b8a202e4c47"</t>
+  </si>
+  <si>
+    <t>diaa</t>
+  </si>
+  <si>
+    <t>kadri</t>
+  </si>
+  <si>
+    <t>22222</t>
+  </si>
+  <si>
+    <t>3232</t>
+  </si>
+  <si>
+    <t>"6591a156d3505b8a202e4c4a"</t>
+  </si>
+  <si>
+    <t>axdo</t>
+  </si>
+  <si>
+    <t>djoudi</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>"6591a2745cbb5e5b2b988168"</t>
   </si>
   <si>
     <t>nabil</t>
@@ -67,53 +101,122 @@
     <t>23244</t>
   </si>
   <si>
-    <t>"6591a156d3505b8a202e4c47"</t>
-  </si>
-  <si>
-    <t>diaa</t>
-  </si>
-  <si>
-    <t>kadri</t>
-  </si>
-  <si>
-    <t>22222</t>
-  </si>
-  <si>
-    <t>3232</t>
-  </si>
-  <si>
-    <t>"6591a156d3505b8a202e4c4a"</t>
-  </si>
-  <si>
-    <t>axdo</t>
-  </si>
-  <si>
-    <t>djoudi</t>
-  </si>
-  <si>
-    <t>11111</t>
-  </si>
-  <si>
-    <t>"6591a2745cbb5e5b2b988168"</t>
-  </si>
-  <si>
     <t>"6591a2745cbb5e5b2b98816b"</t>
   </si>
   <si>
     <t>"6591a2745cbb5e5b2b98816e"</t>
+  </si>
+  <si>
+    <t>"65973be75f3c34552bb2f46a"</t>
+  </si>
+  <si>
+    <t>"65973c0ca3a9f7d98e3f5dbc"</t>
+  </si>
+  <si>
+    <t>"65973c57a3a9f7d98e3f5dd3"</t>
+  </si>
+  <si>
+    <t>"65973cc493aa17adacc0ea28"</t>
+  </si>
+  <si>
+    <t>"65973ceb93aa17adacc0ea2b"</t>
+  </si>
+  <si>
+    <t>"65973d0ed9d6878cd083b6a8"</t>
+  </si>
+  <si>
+    <t>"65973d2de558fcdef983c64e"</t>
+  </si>
+  <si>
+    <t>"65973dadb83be39f51607d9e"</t>
+  </si>
+  <si>
+    <t>"65973dafb83be39f51607da1"</t>
+  </si>
+  <si>
+    <t>"6597414aaeb9485ffcf53ce2"</t>
+  </si>
+  <si>
+    <t>"659c2eb39089769977a56134"</t>
+  </si>
+  <si>
+    <t>NABIL</t>
+  </si>
+  <si>
+    <t>GHEMAM DJERIDI</t>
+  </si>
+  <si>
+    <t>437574</t>
+  </si>
+  <si>
+    <t>"659c2eb49089769977a56137"</t>
+  </si>
+  <si>
+    <t>"659c2eb59089769977a5613a"</t>
+  </si>
+  <si>
+    <t>"659c2eb69089769977a5613d"</t>
+  </si>
+  <si>
+    <t>"659dc6c7cc3786b2787aeaed"</t>
+  </si>
+  <si>
+    <t>adsa</t>
+  </si>
+  <si>
+    <t>"659dc6f5cc3786b2787aeb00"</t>
+  </si>
+  <si>
+    <t>dasfa</t>
+  </si>
+  <si>
+    <t>"65a0326769432e55459b73bf"</t>
+  </si>
+  <si>
+    <t>fafa</t>
+  </si>
+  <si>
+    <t>"65a46e9aa3cf32bad97a6a15"</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>"65a46f4aa3cf32bad97a6ff0"</t>
+  </si>
+  <si>
+    <t>223</t>
+  </si>
+  <si>
+    <t>"65a477c6e2896104054c57ea"</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>"65a84d446e8252428163b5eb"</t>
+  </si>
+  <si>
+    <t>diaa eddine</t>
+  </si>
+  <si>
+    <t>diaakad19@</t>
+  </si>
+  <si>
+    <t>8382383</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -476,11 +579,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.23046875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,10 +613,13 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="I1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A2" t="b">
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -522,156 +633,808 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
         <v>1000</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3">
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>3</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6">
+        <v>6</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A8" t="b">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>1000</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A9" t="b">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>1000</v>
+      </c>
+      <c r="H9">
+        <v>9</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A10" t="b">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>1000</v>
+      </c>
+      <c r="H10">
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A11" t="b">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>1000</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A12" t="b">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>1000</v>
+      </c>
+      <c r="H12">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A13" t="b">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="H13">
+        <v>13</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A14" t="b">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14">
+        <v>14</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A15" t="b">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+      <c r="H15">
+        <v>15</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A16" t="b">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16">
+        <v>1000</v>
+      </c>
+      <c r="H16">
+        <v>16</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" t="b">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>17</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" t="b">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>22</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A19" t="b">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>23</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" t="b">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>24</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" t="b">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>25</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G22" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>28</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>29</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>30</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>31</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>32</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A27">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27">
         <v>2</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>42</v>
+      </c>
+      <c r="F27" t="s">
+        <v>43</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>33</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
         <v>16</v>
       </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-      <c r="G8">
+      <c r="D28" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" t="b">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>34</v>
+      </c>
+      <c r="J28">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>